<commit_message>
updated MTB xlsx file
</commit_message>
<xml_diff>
--- a/data/MTB/MTB_AllInputRefSeqs_20170726.xlsx
+++ b/data/MTB/MTB_AllInputRefSeqs_20170726.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Xiaoyangmiseqdata/MiSeq_20170410/300Test/data/MTB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Xiaoyangmiseqdata/MiSeq_20170410/300TestTeaching/data/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOLD_top_hit!$A$1:$AD$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RDP_midori!$A$1:$S$255</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9856" uniqueCount="1442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9864" uniqueCount="1450">
   <si>
     <t>.id</t>
   </si>
@@ -4360,6 +4360,30 @@
   </si>
   <si>
     <t>Phryganeidae</t>
+  </si>
+  <si>
+    <t>root_prob</t>
+  </si>
+  <si>
+    <t>superkingdom_prob</t>
+  </si>
+  <si>
+    <t>phylum_prob</t>
+  </si>
+  <si>
+    <t>class_prob</t>
+  </si>
+  <si>
+    <t>order_prob</t>
+  </si>
+  <si>
+    <t>family_prob</t>
+  </si>
+  <si>
+    <t>genus_prob</t>
+  </si>
+  <si>
+    <t>species_prob</t>
   </si>
 </sst>
 </file>
@@ -4834,8 +4858,8 @@
   <dimension ref="A1:S255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4862,26 +4886,50 @@
       <c r="D1" t="s">
         <v>213</v>
       </c>
+      <c r="E1" t="s">
+        <v>1442</v>
+      </c>
       <c r="F1" t="s">
         <v>1034</v>
       </c>
+      <c r="G1" t="s">
+        <v>1443</v>
+      </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
+      <c r="I1" t="s">
+        <v>1444</v>
+      </c>
       <c r="J1" t="s">
         <v>14</v>
       </c>
+      <c r="K1" t="s">
+        <v>1445</v>
+      </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
+      <c r="M1" t="s">
+        <v>1446</v>
+      </c>
       <c r="N1" t="s">
         <v>18</v>
       </c>
+      <c r="O1" t="s">
+        <v>1447</v>
+      </c>
       <c r="P1" t="s">
         <v>24</v>
       </c>
+      <c r="Q1" t="s">
+        <v>1448</v>
+      </c>
       <c r="R1" t="s">
         <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1449</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>